<commit_message>
Assessment 2 Files added
</commit_message>
<xml_diff>
--- a/Defect Report/GenericDefectList.xlsx
+++ b/Defect Report/GenericDefectList.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{5B9D3528-E47F-42FF-AADC-31D9E8EB8EB1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:801_{5CCDE88A-A80C-46BC-BC2E-0363EAEE2B0D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="5650" windowWidth="11000" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Dump" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>TestMethod</t>
   </si>
@@ -52,22 +53,20 @@
     <t>DuplicatesFound</t>
   </si>
   <si>
-    <t>loginToAmazon</t>
-  </si>
-  <si>
-    <t>SIT | AmazonPage | loginToAmazon | Enter Password and verify SignIn button is failed in Selenabler Framework</t>
-  </si>
-  <si>
-    <t>1)Navigate to SignIn Page 
-2)Enter Username and continue 
-3)Enter Password and verify SignIn button is failed</t>
+    <t>LanguageChangeToChina</t>
+  </si>
+  <si>
+    <t>SIT | Register | LanguageChangeToChina | SignIn button should be located is failed in Selenabler Framework</t>
+  </si>
+  <si>
+    <t>SignIn button should be located is failed</t>
   </si>
   <si>
     <t>Failure Reason from Selenabler Framework:
-expected [true] but found [false]</t>
-  </si>
-  <si>
-    <t>2023.02.16.16.07.02</t>
+expected [You must be at least 14 years ol] but found [You must be at least 14 years old]</t>
+  </si>
+  <si>
+    <t>2023.07.20.14.34.14</t>
   </si>
   <si>
     <t xml:space="preserve">Chrome </t>
@@ -82,54 +81,35 @@
     <t>0</t>
   </si>
   <si>
-    <t>searchProductOnAmazon</t>
-  </si>
-  <si>
-    <t>SIT | AmazonPage | searchProductOnAmazon | Enter product Name on the search bar is failed in Selenabler Framework</t>
-  </si>
-  <si>
-    <t>1.Navigate to Baby section 
-2.Enter product Name on the search bar is failed</t>
-  </si>
-  <si>
-    <t>2023.02.16.16.07.35</t>
-  </si>
-  <si>
-    <t>addProductToCart</t>
-  </si>
-  <si>
-    <t>SIT | AmazonPage | addProductToCart | Select quantity and add to cart is failed in Selenabler Framework</t>
-  </si>
-  <si>
-    <t>1)Select product after navigating to product page 
-2)Select quantity and add to cart is failed</t>
+    <t>RedirectLinks</t>
+  </si>
+  <si>
+    <t>SIT | Links | RedirectLinks | Application is open is failed in Selenabler Framework</t>
+  </si>
+  <si>
+    <t>Application is open is failed</t>
   </si>
   <si>
     <t>Failure Reason from Selenabler Framework:
-expected [Add to Car] but found [Add to Cart]</t>
-  </si>
-  <si>
-    <t>2023.02.16.16.08.03</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>2023.02.16.16.11.29</t>
+expected [https://www.petitestudionyc.com/collections/buvette-collection] but found [https://www.petitestudionyc.com/collections/business-staples]</t>
+  </si>
+  <si>
+    <t>2023.07.21.00.51.07</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2023.02.16.16.11.47 ,
-2023.02.16.16.07.35</t>
-  </si>
-  <si>
-    <t>2023.02.16.16.12.14 ,
-2023.02.16.16.08.03</t>
+    <t>2023.07.21.00.54.21 ,
+2023.07.21.00.51.07</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2023.07.21.00.58.55 ,
+2023.07.21.00.54.21 ,
+2023.07.21.00.51.07</t>
   </si>
 </sst>
 </file>
@@ -180,12 +160,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -215,7 +192,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>253333</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -253,13 +230,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>253333</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -297,13 +274,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>253333</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -337,24 +314,74 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>253333</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Picture" id="4" name="Picture 1"/>
+        <xdr:cNvPr descr="Picture" id="5" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1301115" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>781018</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr descr="Picture" id="6" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -366,7 +393,89 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1301115" cy="1165860"/>
+          <a:ext cx="1828800" cy="1611630"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>779976</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>138429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr descr="Picture" id="7" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1828800" cy="1611630"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>779976</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr descr="Picture" id="7" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1828800" cy="1611630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -641,23 +750,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.54296875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,17 +798,17 @@
         <v>6</v>
       </c>
     </row>
-    <row ht="60" r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
@@ -712,97 +821,44 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row ht="60" r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row customFormat="1" r="3" spans="1:11" x14ac:dyDescent="0.35"/>
+    <row customFormat="1" r="4" spans="1:11" x14ac:dyDescent="0.35"/>
+    <row customFormat="1" r="5" spans="1:11" x14ac:dyDescent="0.35"/>
+    <row customFormat="1" r="6" spans="1:11" x14ac:dyDescent="0.35"/>
+    <row customFormat="1" r="7" spans="1:11" x14ac:dyDescent="0.35"/>
+    <row r="8">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row ht="60" r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding solution for the assessment
</commit_message>
<xml_diff>
--- a/Defect Report/GenericDefectList.xlsx
+++ b/Defect Report/GenericDefectList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>TestMethod</t>
   </si>
@@ -130,6 +130,22 @@
   <si>
     <t>2023.02.16.16.12.14 ,
 2023.02.16.16.08.03</t>
+  </si>
+  <si>
+    <t>choosing_language_japanese</t>
+  </si>
+  <si>
+    <t>SIT | choosing_language_japanese | choosing_language_japanese | SignIn button should be located is failed in Selenabler Framework</t>
+  </si>
+  <si>
+    <t>SignIn button should be located is failed</t>
+  </si>
+  <si>
+    <t>Failure Reason from Selenabler Framework:
+The language does not changes to English!! expected [true] but found [false]</t>
+  </si>
+  <si>
+    <t>2023.07.20.15.10.26</t>
   </si>
 </sst>
 </file>
@@ -367,6 +383,44 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="1301115" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>781018</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1828800" cy="1611630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -641,7 +695,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
@@ -805,6 +859,35 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>